<commit_message>
security disabled; exception handling added; customer email filed added;
</commit_message>
<xml_diff>
--- a/src/main/resources/pizzaPrice.xlsx
+++ b/src/main/resources/pizzaPrice.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -51,6 +51,21 @@
   </si>
   <si>
     <t>VEGETERIAN</t>
+  </si>
+  <si>
+    <t>Mushroom</t>
+  </si>
+  <si>
+    <t>Cheese</t>
+  </si>
+  <si>
+    <t>calamari</t>
+  </si>
+  <si>
+    <t>DoubleCheese</t>
+  </si>
+  <si>
+    <t>DoubleMushroom</t>
   </si>
 </sst>
 </file>
@@ -93,8 +108,36 @@
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -369,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,6 +469,61 @@
         <v>129</v>
       </c>
     </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
app clean up, delete custom ApplicationContext
</commit_message>
<xml_diff>
--- a/src/main/resources/pizzaPrice.xlsx
+++ b/src/main/resources/pizzaPrice.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IdeaProjects\PizzaService2\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IdeaProjects\pizzaservice\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4656"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -138,6 +138,74 @@
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -157,7 +225,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="A8A8A8"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -415,17 +483,17 @@
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -436,7 +504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -447,7 +515,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -458,7 +526,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -469,7 +537,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -480,7 +548,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -491,7 +559,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -502,7 +570,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -510,10 +578,10 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>13</v>
       </c>

</xml_diff>